<commit_message>
Dodadeni promenite na novata granka courseFeature
</commit_message>
<xml_diff>
--- a/students.csv.xlsx
+++ b/students.csv.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Index</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Stojanovski</t>
+  </si>
+  <si>
+    <t>Aleksandar</t>
+  </si>
+  <si>
+    <t>Velickovski</t>
+  </si>
+  <si>
+    <t>Predrag</t>
+  </si>
+  <si>
+    <t>Spasovski</t>
   </si>
 </sst>
 </file>
@@ -378,7 +390,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,7 +447,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>171027</v>
+        <v>171028</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -456,10 +468,26 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>172064</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>175032</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>

</xml_diff>